<commit_message>
Adds a `loose` mode to sheet cleaning
- This would allow the use of `clean: loose` to only remove
  non-printable characters from the middle of the cell, in addition to
  whitespace at either end of the cell.

- There are a few changes that are somewhat surprising (moving where
  sanitization happens), as the tests that only verified a lack of
  "blowing up" were not getting useful, testable values.
</commit_message>
<xml_diff>
--- a/test/files/parse_clean_with_unicode.xlsx
+++ b/test/files/parse_clean_with_unicode.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10314"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/austin/mess/2021/11/roo/test/files/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B888A32-7A87-544B-9367-3656FB5FAD52}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="14800" windowHeight="8020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,14 +28,15 @@
     <t>Age</t>
   </si>
   <si>
-    <t>  凯   </t>
+    <t xml:space="preserve">
+凯   </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -58,8 +65,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -339,14 +349,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -354,8 +366,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2">

</xml_diff>